<commit_message>
fix(seeder): fix error spreadsheet seeder
Took 22 minutes
</commit_message>
<xml_diff>
--- a/database/seeds/area_alamat.xlsx
+++ b/database/seeds/area_alamat.xlsx
@@ -5,20 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pengelolaan_aset\database\seeds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Web\laragon\www\pengelolaan_aset\database\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89711935-3318-45EA-A804-1F78F1E3390E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11D8370-4E80-48E9-B85F-E0F632DEE499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="area_alamat" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -493,15 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -529,7 +538,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A50" si="0">IF(B3="","","AL" &amp; TEXT(ROW(A3)-1,"0000"))</f>
+        <f t="shared" ref="A3:A47" si="0">IF(B3="","","AL" &amp; TEXT(ROW(A3)-1,"0000"))</f>
         <v>AL0002</v>
       </c>
       <c r="B3" t="s">
@@ -1065,24 +1074,6 @@
       </c>
       <c r="C47" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <f t="shared" si="0"/>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>